<commit_message>
Updated names, added dates from time clock
</commit_message>
<xml_diff>
--- a/Arcadio_Effort_Matrix.xlsx
+++ b/Arcadio_Effort_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/howarat_mail_uc_edu/Documents/Senior-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{764D7873-7837-4CA2-8C86-D736AF11F162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{764D7873-7837-4CA2-8C86-D736AF11F162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FFDA2A1A-5A9A-4E97-9FF1-0C56A9BC24DE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15840" xr2:uid="{4A4CA536-92F5-46DA-A6FB-F2567435B5D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A4CA536-92F5-46DA-A6FB-F2567435B5D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Testing</t>
   </si>
@@ -145,13 +145,55 @@
   </si>
   <si>
     <t>Based on feedback work on fixing bugs seen in Arcadio. Add/Remove features as determined by test and polish project to a final state.</t>
+  </si>
+  <si>
+    <t>October 15th 2020</t>
+  </si>
+  <si>
+    <t>November 15th 2020</t>
+  </si>
+  <si>
+    <t>December 1st 2020</t>
+  </si>
+  <si>
+    <t>Aug 10th 2020</t>
+  </si>
+  <si>
+    <t>February 1st 2021</t>
+  </si>
+  <si>
+    <t>January  15th 2021</t>
+  </si>
+  <si>
+    <t>April 1st 2021</t>
+  </si>
+  <si>
+    <t>April 11th 2021</t>
+  </si>
+  <si>
+    <t>March 15th 2021</t>
+  </si>
+  <si>
+    <t>March 30th 2021</t>
+  </si>
+  <si>
+    <t>March 1st 2021</t>
+  </si>
+  <si>
+    <t>Febrary 1st 2021</t>
+  </si>
+  <si>
+    <t>February 15th 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,21 +291,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,255 +629,307 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E937485-D350-43EF-BC45-0B1AD65B2DD7}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="108" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="4"/>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:7" ht="60">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="9">
+      <c r="E3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:7" ht="90">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="E4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="9">
+      <c r="E6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:7" ht="45">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="E7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="9">
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:7">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="9">
+      <c r="E9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:7" ht="30">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="E10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9">
+      <c r="E11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:7" ht="45">
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="9">
+      <c r="E12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:7" ht="75">
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="9">
+      <c r="E13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:7" ht="60">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="9">
+      <c r="E14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:7" ht="45">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="9">
+      <c r="E15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="6">
         <v>5</v>
       </c>
     </row>

</xml_diff>